<commit_message>
Changes related to New Tag ADJ
</commit_message>
<xml_diff>
--- a/bin/ivt/automation/mappingdoc/NC_IBM_MaPs.xlsx
+++ b/bin/ivt/automation/mappingdoc/NC_IBM_MaPs.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\IVT_Automation_Final\src\ivt\automation\mappingdoc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215D85E0-A68C-47C3-9D09-CD655216FABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{76221296-CC72-4159-BA42-39F3273ECEE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="1" xr2:uid="{48325A19-574D-4D2B-AA7E-D0CEB97E26F2}"/>
+    <workbookView xWindow="1040" yWindow="1020" windowWidth="19180" windowHeight="10200" tabRatio="666" activeTab="1" xr2:uid="{48325A19-574D-4D2B-AA7E-D0CEB97E26F2}"/>
   </bookViews>
   <sheets>
     <sheet name="TagsWithBusinessRules" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,8 @@
     <sheet name="TagMapFinal" sheetId="5" r:id="rId6"/>
     <sheet name="EventMapping" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="159">
   <si>
     <t>NC</t>
   </si>
@@ -1877,19 +1873,19 @@
       <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" style="4" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="66.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="4.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.7265625" style="4" customWidth="1"/>
     <col min="7" max="7" width="33" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="8" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1903,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1918,7 +1914,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
         <v>8</v>
       </c>
@@ -1929,7 +1925,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="55"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
@@ -1938,7 +1934,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="55"/>
       <c r="B5" s="9" t="s">
         <v>7</v>
@@ -1947,7 +1943,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1961,7 +1957,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="56"/>
     </row>
-    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1971,7 +1967,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="56"/>
     </row>
-    <row r="8" spans="1:7" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -2007,7 +2003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -2050,7 +2046,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>74</v>
       </c>
@@ -2061,7 +2057,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>76</v>
       </c>
@@ -2139,101 +2135,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21270FB-1D15-4A2D-84CB-EEA4266FF4AD}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="52" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="52" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2250,177 +2251,177 @@
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
@@ -2438,147 +2439,147 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
         <v>106</v>
       </c>
@@ -2588,22 +2589,22 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>110</v>
       </c>
@@ -2621,19 +2622,19 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="39.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
         <v>38</v>
       </c>
@@ -2651,7 +2652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>40</v>
       </c>
@@ -2673,7 +2674,7 @@
       </c>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -2697,7 +2698,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -2721,7 +2722,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -2745,7 +2746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>-4</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>-3</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>-2</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>-1</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>5</v>
       </c>
@@ -2891,7 +2892,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>6</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>7</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E14" s="19">
         <v>-2</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E15" s="19">
         <v>-1</v>
       </c>
@@ -2971,15 +2972,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -2997,13 +2998,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>2</v>
       </c>
@@ -3011,7 +3012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
         <v>4</v>
       </c>
@@ -3019,7 +3020,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="48" t="s">
         <v>9</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="48" t="s">
         <v>15</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="48" t="s">
         <v>18</v>
       </c>
@@ -3043,7 +3044,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6" s="51" t="s">
         <v>21</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="48" t="s">
         <v>23</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>28</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>32</v>
       </c>
@@ -3112,17 +3113,17 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
@@ -3132,7 +3133,7 @@
       </c>
       <c r="D1" s="61"/>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>115</v>
       </c>
@@ -3149,7 +3150,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
-    <row r="3" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -3166,7 +3167,7 @@
       <c r="F3" s="43"/>
       <c r="G3" s="44"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -3183,7 +3184,7 @@
       <c r="F4" s="43"/>
       <c r="G4" s="44"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="38">
         <v>18</v>
       </c>
@@ -3200,7 +3201,7 @@
       <c r="F5" s="43"/>
       <c r="G5" s="44"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="38">
         <v>13</v>
       </c>
@@ -3217,7 +3218,7 @@
       <c r="F6" s="45"/>
       <c r="G6" s="64"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="38">
         <v>88</v>
       </c>
@@ -3230,7 +3231,7 @@
       <c r="F7" s="43"/>
       <c r="G7" s="65"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="38">
         <v>19</v>
       </c>
@@ -3247,7 +3248,7 @@
       <c r="F8" s="43"/>
       <c r="G8" s="44"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="38">
         <v>99</v>
       </c>
@@ -3260,7 +3261,7 @@
       <c r="F9" s="43"/>
       <c r="G9" s="44"/>
     </row>
-    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="38">
         <v>6</v>
       </c>
@@ -3277,7 +3278,7 @@
       <c r="F10" s="43"/>
       <c r="G10" s="44"/>
     </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="38">
         <v>5</v>
       </c>
@@ -3294,7 +3295,7 @@
       <c r="F11" s="43"/>
       <c r="G11" s="44"/>
     </row>
-    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="38">
         <v>3</v>
       </c>
@@ -3311,7 +3312,7 @@
       <c r="F12" s="43"/>
       <c r="G12" s="44"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="38">
         <v>4</v>
       </c>
@@ -3328,7 +3329,7 @@
       <c r="F13" s="43"/>
       <c r="G13" s="44"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="38">
         <v>23</v>
       </c>
@@ -3345,7 +3346,7 @@
       <c r="F14" s="43"/>
       <c r="G14" s="44"/>
     </row>
-    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="38">
         <v>8</v>
       </c>
@@ -3362,7 +3363,7 @@
       <c r="F15" s="43"/>
       <c r="G15" s="44"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="38">
         <v>21</v>
       </c>
@@ -3379,7 +3380,7 @@
       <c r="F16" s="43"/>
       <c r="G16" s="44"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="38">
         <v>20</v>
       </c>
@@ -3396,7 +3397,7 @@
       <c r="F17" s="43"/>
       <c r="G17" s="44"/>
     </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="38">
         <v>7</v>
       </c>
@@ -3413,7 +3414,7 @@
       <c r="F18" s="43"/>
       <c r="G18" s="44"/>
     </row>
-    <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="38">
         <v>9</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>22</v>
       </c>
@@ -3542,7 +3543,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="38"/>
       <c r="B28" s="39"/>
       <c r="C28" s="3"/>

</xml_diff>

<commit_message>
EVTOTAL and TUKLATEFEE MErged
</commit_message>
<xml_diff>
--- a/bin/ivt/automation/mappingdoc/NC_IBM_MaPs.xlsx
+++ b/bin/ivt/automation/mappingdoc/NC_IBM_MaPs.xlsx
@@ -5,21 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204747\IVT_WorkSpace\IVT_Automation_Main_project\src\ivt\automation\mappingdoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\208394\IdeaProjects\Invoice_NCIBM_Auto\src\ivt\automation\testData\MDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B064E796-D337-4BAF-8620-FF907C6F87E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC157E6-DE7D-426C-8B3F-68B053CA256D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="20490" windowHeight="10920" tabRatio="666" activeTab="1" xr2:uid="{48325A19-574D-4D2B-AA7E-D0CEB97E26F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" firstSheet="1" activeTab="5" xr2:uid="{48325A19-574D-4D2B-AA7E-D0CEB97E26F2}"/>
   </bookViews>
   <sheets>
-    <sheet name="TagsWithBusinessRules" sheetId="1" r:id="rId1"/>
-    <sheet name="IBMNCTAG" sheetId="7" r:id="rId2"/>
+    <sheet name="IBMNCTAG" sheetId="7" r:id="rId1"/>
+    <sheet name="TagsWithBusinessRules" sheetId="1" r:id="rId2"/>
     <sheet name="NCTAG" sheetId="3" r:id="rId3"/>
-    <sheet name="IBMTAG" sheetId="4" r:id="rId4"/>
-    <sheet name="TaxCodeMapping" sheetId="2" r:id="rId5"/>
-    <sheet name="TagMapFinal" sheetId="5" r:id="rId6"/>
-    <sheet name="EventMapping" sheetId="6" r:id="rId7"/>
+    <sheet name="BusinessRulesTag" sheetId="9" r:id="rId4"/>
+    <sheet name="IBMBrTag" sheetId="10" r:id="rId5"/>
+    <sheet name="TaxMap" sheetId="12" r:id="rId6"/>
+    <sheet name="BREventMapName" sheetId="11" r:id="rId7"/>
+    <sheet name="IBMTAG" sheetId="4" r:id="rId8"/>
+    <sheet name="TaxCodeMapping" sheetId="2" r:id="rId9"/>
+    <sheet name="TagMapFinal" sheetId="5" r:id="rId10"/>
+    <sheet name="EventMapping" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="297">
   <si>
     <t>NC</t>
   </si>
@@ -1022,12 +1026,426 @@
   <si>
     <t>TagNames</t>
   </si>
+  <si>
+    <t>EVTOTAL_41</t>
+  </si>
+  <si>
+    <t>EVTOTAL_3</t>
+  </si>
+  <si>
+    <t>EVTOTAL_4</t>
+  </si>
+  <si>
+    <t>EVTOTAL_5</t>
+  </si>
+  <si>
+    <t>EVTOTAL_6</t>
+  </si>
+  <si>
+    <t>EVTOTAL_7</t>
+  </si>
+  <si>
+    <t>EVTOTAL_8</t>
+  </si>
+  <si>
+    <t>EVTOTAL_9</t>
+  </si>
+  <si>
+    <t>EVTOTAL_10</t>
+  </si>
+  <si>
+    <t>EVTOTAL_42</t>
+  </si>
+  <si>
+    <t>EVTOTAL_16</t>
+  </si>
+  <si>
+    <t>EVTOTAL_22</t>
+  </si>
+  <si>
+    <t>EVTOTAL_23</t>
+  </si>
+  <si>
+    <t>EVTOTAL_11</t>
+  </si>
+  <si>
+    <t>EVTOTAL_12</t>
+  </si>
+  <si>
+    <t>EVTOTAL_13</t>
+  </si>
+  <si>
+    <t>EVTOTAL_24</t>
+  </si>
+  <si>
+    <t>EVTOTAL_40</t>
+  </si>
+  <si>
+    <t>EVTOTAL_43</t>
+  </si>
+  <si>
+    <t>EVTOTAL_44</t>
+  </si>
+  <si>
+    <t>EVTOTAL_45</t>
+  </si>
+  <si>
+    <t>EVTOTAL_55</t>
+  </si>
+  <si>
+    <t>EVTOTAL_57</t>
+  </si>
+  <si>
+    <t>EVTOTAL_58</t>
+  </si>
+  <si>
+    <t>EVTOTAL_59</t>
+  </si>
+  <si>
+    <t>EVTOTAL_18</t>
+  </si>
+  <si>
+    <t>EVTOTAL_15</t>
+  </si>
+  <si>
+    <t>EVTOTAL_14</t>
+  </si>
+  <si>
+    <t>EVTOTAL_1</t>
+  </si>
+  <si>
+    <t>EVTOTAL_19</t>
+  </si>
+  <si>
+    <t>EVTOTAL_20</t>
+  </si>
+  <si>
+    <t>EVTOTAL_21</t>
+  </si>
+  <si>
+    <t>EVTOTAL_17</t>
+  </si>
+  <si>
+    <t>EVTOTAL_2</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>BrTags</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT_1_3102</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT_1_3103</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT_&lt;1_3104</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT</t>
+  </si>
+  <si>
+    <t>TUKUSAGESUMMARY Minutes</t>
+  </si>
+  <si>
+    <t>TUKUSAGESUMMARY Text Messages</t>
+  </si>
+  <si>
+    <t>TUKUSAGESUMMARY Media Messages</t>
+  </si>
+  <si>
+    <t>TUKUSAGESUMMARY Data</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT_3102</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT_3103</t>
+  </si>
+  <si>
+    <t>O2RTDTOTALEVT_3104</t>
+  </si>
+  <si>
+    <t>servicetype</t>
+  </si>
+  <si>
+    <t>allowancetype</t>
+  </si>
+  <si>
+    <t>allowanceInitialAmt</t>
+  </si>
+  <si>
+    <t>allowanceConsumedAmt</t>
+  </si>
+  <si>
+    <t>allowanceStart date</t>
+  </si>
+  <si>
+    <t>end dates</t>
+  </si>
+  <si>
+    <t>count of one off MMS or Data allowance</t>
+  </si>
+  <si>
+    <t>Total usage</t>
+  </si>
+  <si>
+    <t>remaining usage</t>
+  </si>
+  <si>
+    <t>total usage discounted</t>
+  </si>
+  <si>
+    <t>total money discounted</t>
+  </si>
+  <si>
+    <t>total amount of usage in this period (discounted and not discounted)</t>
+  </si>
+  <si>
+    <t>total usage discounted in this bill</t>
+  </si>
+  <si>
+    <t>total money discounted in this bill</t>
+  </si>
+  <si>
+    <t>usage allowance</t>
+  </si>
+  <si>
+    <t>allowance available</t>
+  </si>
+  <si>
+    <t>Budget Centre</t>
+  </si>
+  <si>
+    <t>EU Data</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_41</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_3</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_4</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_5</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_6</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_42</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_9</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_10</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_8</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_7</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_16</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_22</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_23</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_11</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_13</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_18</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_24</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_1</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_44</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_20</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_40</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_11</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_55</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_12</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_57</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_16</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_43</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_19</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_45</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_21</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_58</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_17</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_59</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_2</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_15</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_13</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_12</t>
+  </si>
+  <si>
+    <t>IBM_EVTOTAL_22</t>
+  </si>
+  <si>
+    <t>NC_EVTOTAL_14</t>
+  </si>
+  <si>
+    <t>IBM_</t>
+  </si>
+  <si>
+    <t>NC_</t>
+  </si>
+  <si>
+    <t>IBM Do not have Tags</t>
+  </si>
+  <si>
+    <t>NC Do Not have Tags</t>
+  </si>
+  <si>
+    <t>OTCTAXCODE</t>
+  </si>
+  <si>
+    <t>BSTARTOTCLIST</t>
+  </si>
+  <si>
+    <t>BSTARTOTC</t>
+  </si>
+  <si>
+    <t>BENDOTC</t>
+  </si>
+  <si>
+    <t>BENDOTCLIST</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>CUK-3005</t>
+  </si>
+  <si>
+    <t>CUK-3008</t>
+  </si>
+  <si>
+    <t>CUK-3004</t>
+  </si>
+  <si>
+    <t>CUK-3010</t>
+  </si>
+  <si>
+    <t>CUK-3009</t>
+  </si>
+  <si>
+    <t>CUK-3006</t>
+  </si>
+  <si>
+    <t>CUK-3002</t>
+  </si>
+  <si>
+    <t>CUK-3007</t>
+  </si>
+  <si>
+    <t>CUK-3003</t>
+  </si>
+  <si>
+    <t>CUK--4</t>
+  </si>
+  <si>
+    <t>CUK--3</t>
+  </si>
+  <si>
+    <t>CUK--2</t>
+  </si>
+  <si>
+    <t>CUK--1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1105,6 +1523,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1388,7 +1812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1523,6 +1947,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1558,6 +2001,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1872,14 +2321,688 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21270FB-1D15-4A2D-84CB-EEA4266FF4AD}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0727881-AA9D-4FC6-934D-9D7EDCD17013}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17728A01-742B-4C18-BB96-9C461D72396D}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="68"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+    </row>
+    <row r="3" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="40">
+        <v>59</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="40">
+        <v>24</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38">
+        <v>18</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="40">
+        <v>12</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="38">
+        <v>13</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="40">
+        <v>11</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="69"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="71"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
+        <v>88</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="72"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>19</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="40">
+        <v>43</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>99</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38">
+        <v>6</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="40">
+        <v>41</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>5</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="40">
+        <v>41</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>3</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="40">
+        <v>41</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38">
+        <v>4</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="40">
+        <v>41</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38">
+        <v>23</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="40">
+        <v>16</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+    </row>
+    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38">
+        <v>8</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="40">
+        <v>42</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38">
+        <v>21</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="40">
+        <v>45</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38">
+        <v>20</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="40">
+        <v>44</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+    </row>
+    <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38">
+        <v>7</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="40">
+        <v>42</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="42"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
+    </row>
+    <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38">
+        <v>9</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="40">
+        <v>42</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="42"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="44"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>10</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="40">
+        <v>42</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>11</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="40">
+        <v>40</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <v>12</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="40">
+        <v>55</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <v>16</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="40">
+        <v>57</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="38">
+        <v>17</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="40">
+        <v>58</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="38">
+        <v>14</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="40">
+        <v>22</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="38">
+        <v>15</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="40">
+        <v>13</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="38">
+        <v>22</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27" s="40">
+        <v>16</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="G6:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C962B76-521D-4DAC-A2FC-A4C6198CF0B7}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="4" customWidth="1"/>
     <col min="2" max="2" width="66.28515625" style="4" customWidth="1"/>
@@ -1921,7 +3044,7 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="62" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1932,7 +3055,7 @@
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1941,7 +3064,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
@@ -1953,7 +3076,7 @@
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="61" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1961,17 +3084,17 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="56"/>
+      <c r="F6" s="63"/>
     </row>
     <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="54"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="10"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="56"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:7" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -2136,110 +3259,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21270FB-1D15-4A2D-84CB-EEA4266FF4AD}">
-  <dimension ref="A1:A17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2433,6 +3452,1082 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47633404-1665-4C13-8263-A2D1A4F99154}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H6" t="s">
+        <v>220</v>
+      </c>
+      <c r="I6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J6" t="s">
+        <v>222</v>
+      </c>
+      <c r="K6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="56" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>269</v>
+      </c>
+      <c r="B25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47475F54-1500-4228-BBC8-189B864F10A1}">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D93E0B-D1D4-4D76-A35C-0435198D0E3C}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="55"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="73" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="73">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="73" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="73" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="73" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="73" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="73" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="73" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="73">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="19">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A72517-6C94-491C-9632-83FEED170E98}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="55"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>241</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B24" s="58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>250</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="B31" s="57" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="B33" s="57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="56" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="58" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="56" t="s">
+        <v>258</v>
+      </c>
+      <c r="B35" s="57" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="B36" s="58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
+        <v>259</v>
+      </c>
+      <c r="B37" s="58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="B38" s="58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="B39" s="58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{781B61E8-10B3-4DA8-B07A-D97BE3ACCF84}">
   <dimension ref="A1:A35"/>
   <sheetViews>
@@ -2615,12 +4710,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6F2332-EB2F-410F-A965-AD8DE62F93ED}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,19 +4731,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
       <c r="D1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
       <c r="H1" s="12" t="s">
         <v>33</v>
       </c>
@@ -2989,576 +5084,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0727881-AA9D-4FC6-934D-9D7EDCD17013}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17728A01-742B-4C18-BB96-9C461D72396D}">
-  <dimension ref="A1:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" s="61"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-    </row>
-    <row r="3" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38">
-        <v>2</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="40">
-        <v>59</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38">
-        <v>1</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="40">
-        <v>24</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38">
-        <v>18</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="40">
-        <v>12</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="38">
-        <v>13</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="40">
-        <v>11</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="64"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38">
-        <v>88</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="65"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38">
-        <v>19</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="40">
-        <v>43</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38">
-        <v>99</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38">
-        <v>6</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="40">
-        <v>41</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
-    </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
-        <v>5</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="40">
-        <v>41</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
-    </row>
-    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38">
-        <v>3</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="40">
-        <v>41</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
-    </row>
-    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38">
-        <v>4</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="40">
-        <v>41</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38">
-        <v>23</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="40">
-        <v>16</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
-    </row>
-    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38">
-        <v>8</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="40">
-        <v>42</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38">
-        <v>21</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="40">
-        <v>45</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38">
-        <v>20</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="40">
-        <v>44</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
-    </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38">
-        <v>7</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="40">
-        <v>42</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
-    </row>
-    <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38">
-        <v>9</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="C19" s="40">
-        <v>42</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="38">
-        <v>10</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" s="40">
-        <v>42</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
-        <v>11</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="C21" s="40">
-        <v>40</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
-        <v>12</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="40">
-        <v>55</v>
-      </c>
-      <c r="D22" s="41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
-        <v>16</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="C23" s="40">
-        <v>57</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
-        <v>17</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="40">
-        <v>58</v>
-      </c>
-      <c r="D24" s="41" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
-        <v>14</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="C25" s="40">
-        <v>22</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
-        <v>15</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="40">
-        <v>13</v>
-      </c>
-      <c r="D26" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="38">
-        <v>22</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="C27" s="40">
-        <v>16</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="47" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="G6:G7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Code Cleaning and Merge
</commit_message>
<xml_diff>
--- a/bin/ivt/automation/mappingdoc/NC_IBM_MaPs.xlsx
+++ b/bin/ivt/automation/mappingdoc/NC_IBM_MaPs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\208394\IdeaProjects\Invoice_NCIBM_Auto\src\ivt\automation\testData\MDoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\094539\Desktop\IVT DOCS\Code\IVT_Automation_WorkSapce\IVT_Automation_Main_project\src\ivt\automation\mappingdoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC157E6-DE7D-426C-8B3F-68B053CA256D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E8A7A1-8F76-4454-8EF0-5D5CCADEFB8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" firstSheet="1" activeTab="5" xr2:uid="{48325A19-574D-4D2B-AA7E-D0CEB97E26F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="666" xr2:uid="{48325A19-574D-4D2B-AA7E-D0CEB97E26F2}"/>
   </bookViews>
   <sheets>
     <sheet name="IBMNCTAG" sheetId="7" r:id="rId1"/>
@@ -1966,6 +1966,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2001,12 +2007,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2324,97 +2324,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21270FB-1D15-4A2D-84CB-EEA4266FF4AD}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="53" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="52" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
         <v>100</v>
       </c>
@@ -2430,13 +2430,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>2</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
         <v>4</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="48" t="s">
         <v>9</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="48" t="s">
         <v>15</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="48" t="s">
         <v>18</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A6" s="51" t="s">
         <v>21</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="48" t="s">
         <v>23</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A8" s="49" t="s">
         <v>74</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="49" t="s">
         <v>76</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="49" t="s">
         <v>30</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="48" t="s">
         <v>28</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="48" t="s">
         <v>32</v>
       </c>
@@ -2545,27 +2545,27 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="67" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="70"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>115</v>
       </c>
@@ -2582,7 +2582,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
-    <row r="3" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="38">
         <v>2</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="F3" s="43"/>
       <c r="G3" s="44"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="F4" s="43"/>
       <c r="G4" s="44"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="38">
         <v>18</v>
       </c>
@@ -2633,7 +2633,7 @@
       <c r="F5" s="43"/>
       <c r="G5" s="44"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="38">
         <v>13</v>
       </c>
@@ -2646,11 +2646,11 @@
       <c r="D6" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="69"/>
+      <c r="E6" s="71"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="71"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="73"/>
+    </row>
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="38">
         <v>88</v>
       </c>
@@ -2659,11 +2659,11 @@
       </c>
       <c r="C7" s="40"/>
       <c r="D7" s="41"/>
-      <c r="E7" s="70"/>
+      <c r="E7" s="72"/>
       <c r="F7" s="43"/>
-      <c r="G7" s="72"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="74"/>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="38">
         <v>19</v>
       </c>
@@ -2680,7 +2680,7 @@
       <c r="F8" s="43"/>
       <c r="G8" s="44"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="38">
         <v>99</v>
       </c>
@@ -2693,7 +2693,7 @@
       <c r="F9" s="43"/>
       <c r="G9" s="44"/>
     </row>
-    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="38">
         <v>6</v>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="F10" s="43"/>
       <c r="G10" s="44"/>
     </row>
-    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="38">
         <v>5</v>
       </c>
@@ -2727,7 +2727,7 @@
       <c r="F11" s="43"/>
       <c r="G11" s="44"/>
     </row>
-    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="38">
         <v>3</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="F12" s="43"/>
       <c r="G12" s="44"/>
     </row>
-    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="38">
         <v>4</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="F13" s="43"/>
       <c r="G13" s="44"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="38">
         <v>23</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="F14" s="43"/>
       <c r="G14" s="44"/>
     </row>
-    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="38">
         <v>8</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="F15" s="43"/>
       <c r="G15" s="44"/>
     </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="38">
         <v>21</v>
       </c>
@@ -2812,7 +2812,7 @@
       <c r="F16" s="43"/>
       <c r="G16" s="44"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="38">
         <v>20</v>
       </c>
@@ -2829,7 +2829,7 @@
       <c r="F17" s="43"/>
       <c r="G17" s="44"/>
     </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="38">
         <v>7</v>
       </c>
@@ -2846,7 +2846,7 @@
       <c r="F18" s="43"/>
       <c r="G18" s="44"/>
     </row>
-    <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="38">
         <v>9</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="F19" s="43"/>
       <c r="G19" s="44"/>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="38">
         <v>10</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="38">
         <v>11</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="38">
         <v>12</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="38">
         <v>16</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="38">
         <v>17</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="38">
         <v>14</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="38">
         <v>15</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="38">
         <v>22</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="38"/>
       <c r="B28" s="39"/>
       <c r="C28" s="3"/>
@@ -3002,19 +3002,19 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" style="4" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="66.26953125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="4.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="31.7265625" style="4" customWidth="1"/>
     <col min="7" max="7" width="33" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="8" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -3043,8 +3043,8 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+    <row r="3" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -3054,8 +3054,8 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+    <row r="4" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="64"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -3063,8 +3063,8 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+    <row r="5" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="64"/>
       <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
@@ -3072,11 +3072,11 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="63" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -3084,19 +3084,19 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="63"/>
-    </row>
-    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="65"/>
+    </row>
+    <row r="7" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="61"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="10"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="63"/>
-    </row>
-    <row r="8" spans="1:7" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="65"/>
+    </row>
+    <row r="8" spans="1:7" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="162.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="306" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="306" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>74</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>76</v>
       </c>
@@ -3197,7 +3197,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>30</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -3223,7 +3223,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>30</v>
       </c>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
@@ -3271,177 +3271,177 @@
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
@@ -3459,21 +3459,21 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>193</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>199</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="54" t="s">
         <v>159</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="54" t="s">
         <v>168</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="54" t="s">
         <v>169</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="56" t="s">
         <v>172</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="56" t="s">
         <v>173</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="56" t="s">
         <v>174</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="56" t="s">
         <v>170</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="56" t="s">
         <v>175</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="56" t="s">
         <v>176</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="56" t="s">
         <v>177</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="56" t="s">
         <v>178</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="56" t="s">
         <v>179</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="56" t="s">
         <v>180</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
         <v>181</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
         <v>182</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
         <v>183</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="60" t="s">
         <v>4</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>270</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="60" t="s">
         <v>269</v>
       </c>
@@ -3765,112 +3765,112 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="54" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="54" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="54" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="56" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="56" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="56" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="56" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="56" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="56" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="56" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="56" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="56" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="56" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="56" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="56" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="60" t="s">
         <v>4</v>
       </c>
@@ -3884,19 +3884,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D93E0B-D1D4-4D76-A35C-0435198D0E3C}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>40</v>
       </c>
@@ -3908,128 +3908,128 @@
       </c>
       <c r="D1" s="55"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="s">
         <v>276</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="73">
+      <c r="C2" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="61" t="s">
         <v>277</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="61">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="61" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="73">
+      <c r="C4" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="73" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="61" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="73">
+      <c r="C7" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="61" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="73">
+      <c r="C8" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="61" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="73">
+      <c r="C9" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="73">
+      <c r="C10" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="61" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="73">
+      <c r="C11" s="61">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="61" t="s">
         <v>283</v>
       </c>
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="73">
+      <c r="C12" s="61">
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>284</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>285</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>286</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>287</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>288</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>289</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
         <v>290</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="19" t="s">
         <v>291</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="19" t="s">
         <v>292</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
         <v>293</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="19" t="s">
         <v>294</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="19" t="s">
         <v>295</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>296</v>
       </c>
@@ -4186,14 +4186,14 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="55"/>
+    <col min="1" max="1" width="16.453125" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.453125" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="54" t="s">
         <v>225</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="54" t="s">
         <v>226</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
         <v>227</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="54" t="s">
         <v>228</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="54" t="s">
         <v>229</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="54" t="s">
         <v>230</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="55" t="s">
         <v>231</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="55" t="s">
         <v>232</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="55" t="s">
         <v>233</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="54" t="s">
         <v>234</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="54" t="s">
         <v>235</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="56" t="s">
         <v>236</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="56" t="s">
         <v>237</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="56" t="s">
         <v>238</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="56" t="s">
         <v>239</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="56" t="s">
         <v>261</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="56" t="s">
         <v>240</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="56" t="s">
         <v>241</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="56" t="s">
         <v>242</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
         <v>243</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
         <v>244</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
         <v>245</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="56" t="s">
         <v>246</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
         <v>247</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="56" t="s">
         <v>248</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="56" t="s">
         <v>249</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="56" t="s">
         <v>250</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="56" t="s">
         <v>251</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="56" t="s">
         <v>252</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="56" t="s">
         <v>253</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="56" t="s">
         <v>254</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="56" t="s">
         <v>255</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="56" t="s">
         <v>256</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="56" t="s">
         <v>257</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="56" t="s">
         <v>258</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="56" t="s">
         <v>260</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="56" t="s">
         <v>259</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="56" t="s">
         <v>262</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="56" t="s">
         <v>263</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="56" t="s">
         <v>264</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="56" t="s">
         <v>265</v>
       </c>
@@ -4535,172 +4535,172 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
         <v>110</v>
       </c>
@@ -4718,37 +4718,37 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="39.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
       <c r="H1" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>40</v>
       </c>
@@ -4770,7 +4770,7 @@
       </c>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="16">
         <v>1</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>-4</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>-3</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>-2</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>-1</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>5</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>6</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>7</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E14" s="19">
         <v>-2</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E15" s="19">
         <v>-1</v>
       </c>
@@ -5068,15 +5068,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>

</xml_diff>